<commit_message>
dynamic sink term added
</commit_message>
<xml_diff>
--- a/masterProject/Cases_simplified_model.xlsx
+++ b/masterProject/Cases_simplified_model.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="107">
   <si>
     <t>comments</t>
   </si>
@@ -94,13 +94,16 @@
     <t>Tfuel</t>
   </si>
   <si>
+    <t>T_whole</t>
+  </si>
+  <si>
+    <t>Xbed</t>
+  </si>
+  <si>
     <t>P_gas</t>
   </si>
   <si>
-    <t>P_heat</t>
-  </si>
-  <si>
-    <t>nboil</t>
+    <t>P_fuel</t>
   </si>
   <si>
     <t>xH2O_G_wet</t>
@@ -349,6 +352,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -632,10 +636,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AO4"/>
+  <dimension ref="A1:AP4"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A20" activeCellId="0" sqref="A20"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="P1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AD1" activeCellId="0" sqref="AD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -648,11 +652,11 @@
     <col collapsed="false" hidden="false" max="13" min="13" style="1" width="11.5714285714286"/>
     <col collapsed="false" hidden="false" max="19" min="14" style="0" width="11.5714285714286"/>
     <col collapsed="false" hidden="false" max="20" min="20" style="2" width="11.5714285714286"/>
-    <col collapsed="false" hidden="false" max="37" min="21" style="0" width="11.5714285714286"/>
-    <col collapsed="false" hidden="false" max="38" min="38" style="0" width="12.8622448979592"/>
-    <col collapsed="false" hidden="false" max="39" min="39" style="0" width="11.5714285714286"/>
-    <col collapsed="false" hidden="false" max="40" min="40" style="0" width="14.1479591836735"/>
-    <col collapsed="false" hidden="false" max="1025" min="41" style="0" width="11.5714285714286"/>
+    <col collapsed="false" hidden="false" max="38" min="21" style="0" width="11.5714285714286"/>
+    <col collapsed="false" hidden="false" max="39" min="39" style="0" width="12.8622448979592"/>
+    <col collapsed="false" hidden="false" max="40" min="40" style="0" width="11.5714285714286"/>
+    <col collapsed="false" hidden="false" max="41" min="41" style="0" width="14.1479591836735"/>
+    <col collapsed="false" hidden="false" max="1025" min="42" style="0" width="11.5714285714286"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -779,121 +783,124 @@
       <c r="AO1" s="0" t="s">
         <v>40</v>
       </c>
+      <c r="AP1" s="0" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="H2" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="I2" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="J2" s="11" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="K2" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="L2" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="M2" s="10" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="N2" s="0" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="O2" s="0" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="P2" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="Q2" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="R2" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="S2" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="T2" s="11" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="U2" s="0" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="V2" s="0" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="W2" s="0" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="X2" s="0" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="Y2" s="0" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="Z2" s="0" t="s">
         <v>50</v>
       </c>
       <c r="AA2" s="0" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="AB2" s="0" t="s">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="AC2" s="0" t="s">
         <v>51</v>
       </c>
       <c r="AD2" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="AE2" s="0" t="s">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="AF2" s="0" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="AG2" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="AH2" s="0" t="s">
         <v>53</v>
       </c>
       <c r="AI2" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="AJ2" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="AK2" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="AL2" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="AM2" s="0" t="s">
         <v>54</v>
@@ -904,10 +911,13 @@
       <c r="AO2" s="0" t="s">
         <v>56</v>
       </c>
+      <c r="AP2" s="0" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>0</v>
@@ -982,22 +992,22 @@
         <v>40</v>
       </c>
       <c r="Z3" s="0" t="n">
+        <v>500</v>
+      </c>
+      <c r="AA3" s="0" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="AB3" s="0" t="n">
         <v>10</v>
       </c>
-      <c r="AA3" s="0" t="n">
+      <c r="AC3" s="0" t="n">
         <v>70</v>
-      </c>
-      <c r="AB3" s="0" t="n">
-        <v>0.89</v>
-      </c>
-      <c r="AC3" s="0" t="n">
-        <v>0.55</v>
       </c>
       <c r="AD3" s="0" t="n">
         <v>0.55</v>
       </c>
       <c r="AE3" s="0" t="n">
-        <v>1.2</v>
+        <v>0.55</v>
       </c>
       <c r="AF3" s="0" t="n">
         <v>1.2</v>
@@ -1006,27 +1016,30 @@
         <v>1.2</v>
       </c>
       <c r="AH3" s="0" t="n">
-        <v>0.65</v>
+        <v>1.2</v>
       </c>
       <c r="AI3" s="0" t="n">
+        <v>0.55</v>
+      </c>
+      <c r="AJ3" s="0" t="n">
         <v>2.6</v>
       </c>
-      <c r="AJ3" s="0" t="n">
+      <c r="AK3" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="AK3" s="0" t="n">
-        <v>0.5</v>
-      </c>
       <c r="AL3" s="0" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="AM3" s="0" t="n">
         <v>0.15</v>
       </c>
-      <c r="AM3" s="0" t="n">
+      <c r="AN3" s="0" t="n">
         <v>0.02</v>
       </c>
-      <c r="AN3" s="0" t="n">
+      <c r="AO3" s="0" t="n">
         <v>0.525</v>
       </c>
-      <c r="AO3" s="0" t="n">
+      <c r="AP3" s="0" t="n">
         <v>2610</v>
       </c>
     </row>
@@ -1067,168 +1080,168 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="8" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="F1" s="8" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="G1" s="8" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="H1" s="8" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="I1" s="12" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="J1" s="12" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="K1" s="12" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="L1" s="12" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="M1" s="12" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="N1" s="12" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="O1" s="13" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="P1" s="13" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="Q1" s="13" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="R1" s="13" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="S1" s="14" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="T1" s="14" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="U1" s="14" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="V1" s="14" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="W1" s="14" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="X1" s="14" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="Y1" s="15" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="Z1" s="15" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="AA1" s="15" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B2" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="F2" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="G2" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="H2" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="I2" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="J2" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="K2" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="L2" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="M2" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="N2" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="O2" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="P2" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q2" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="R2" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="S2" s="0" t="s">
         <v>50</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="T2" s="0" t="s">
         <v>50</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="U2" s="0" t="s">
         <v>50</v>
       </c>
-      <c r="E2" s="0" t="s">
+      <c r="V2" s="0" t="s">
         <v>50</v>
       </c>
-      <c r="F2" s="0" t="s">
+      <c r="W2" s="0" t="s">
         <v>50</v>
       </c>
-      <c r="G2" s="0" t="s">
+      <c r="X2" s="0" t="s">
         <v>50</v>
       </c>
-      <c r="H2" s="0" t="s">
-        <v>86</v>
-      </c>
-      <c r="I2" s="0" t="s">
-        <v>85</v>
-      </c>
-      <c r="J2" s="0" t="s">
-        <v>50</v>
-      </c>
-      <c r="K2" s="0" t="s">
-        <v>50</v>
-      </c>
-      <c r="L2" s="0" t="s">
-        <v>50</v>
-      </c>
-      <c r="M2" s="0" t="s">
-        <v>50</v>
-      </c>
-      <c r="N2" s="0" t="s">
-        <v>50</v>
-      </c>
-      <c r="O2" s="0" t="s">
-        <v>50</v>
-      </c>
-      <c r="P2" s="0" t="s">
-        <v>50</v>
-      </c>
-      <c r="Q2" s="0" t="s">
-        <v>50</v>
-      </c>
-      <c r="R2" s="0" t="s">
-        <v>50</v>
-      </c>
-      <c r="S2" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="T2" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="U2" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="V2" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="W2" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="X2" s="0" t="s">
-        <v>49</v>
-      </c>
       <c r="Y2" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="Z2" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="AA2" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -1260,33 +1273,33 @@
   <sheetData>
     <row r="1" customFormat="false" ht="24.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="16" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C1" s="16" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D1" s="16" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="E1" s="16" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="F1" s="16" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="G1" s="16" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="H1" s="16" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="I1" s="16" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="16" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B2" s="17" t="n">
         <v>0.035</v>
@@ -1302,7 +1315,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="16" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B3" s="17" t="n">
         <v>0.518</v>
@@ -1332,7 +1345,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="16" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B4" s="17" t="n">
         <v>0.06</v>
@@ -1362,7 +1375,7 @@
     </row>
     <row r="5" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="16" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B5" s="17" t="n">
         <v>0.381</v>
@@ -1392,7 +1405,7 @@
     </row>
     <row r="6" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="16" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B6" s="17" t="n">
         <v>0.0054</v>
@@ -1422,7 +1435,7 @@
     </row>
     <row r="7" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="16" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B7" s="17" t="n">
         <v>0.0009</v>
@@ -1452,7 +1465,7 @@
     </row>
     <row r="8" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="16" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B8" s="17" t="n">
         <v>19.738</v>
@@ -1541,7 +1554,7 @@
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B31" s="0" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1575,7 +1588,7 @@
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B33" s="0" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C33" s="0" t="n">
         <v>40.58</v>
@@ -1607,7 +1620,7 @@
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B34" s="0" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C34" s="0" t="n">
         <v>36.32</v>
@@ -1639,7 +1652,7 @@
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B35" s="0" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C35" s="0" t="n">
         <v>27.51</v>

</xml_diff>